<commit_message>
còn đúng css thôi
</commit_message>
<xml_diff>
--- a/giangvien/bangdiem.xlsx
+++ b/giangvien/bangdiem.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Msv</t>
   </si>
@@ -42,15 +42,6 @@
   </si>
   <si>
     <t>PHP nâng cao</t>
-  </si>
-  <si>
-    <t>quan</t>
-  </si>
-  <si>
-    <t>Lập trình với PHP</t>
-  </si>
-  <si>
-    <t>Xây dựng hệ thống</t>
   </si>
 </sst>
 </file>
@@ -415,16 +406,16 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="2" max="2" width="15.281982" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="21.137695" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="15.281982" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -471,52 +462,6 @@
       </c>
       <c r="G2" s="2">
         <v>8.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>